<commit_message>
BUG: read_excel forward-filling MI names (#38517)
Closes https://github.com/pandas-dev/pandas/issues/34673
</commit_message>
<xml_diff>
--- a/pandas/tests/io/data/excel/testmultiindex.xlsx
+++ b/pandas/tests/io/data/excel/testmultiindex.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Beano\Repositories\pandas\pandas\tests\io\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewzeitlin/Code/contrib/pandas-mzeitlin11/pandas/tests/io/data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62484658-60B6-4AFE-9718-E1BB2EECC154}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CD6934-D64C-2943-AF8E-713547E05FF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="single_column_name" sheetId="9" r:id="rId1"/>
@@ -20,9 +20,12 @@
     <sheet name="mi_column_name" sheetId="4" r:id="rId5"/>
     <sheet name="name_with_int" sheetId="12" r:id="rId6"/>
     <sheet name="mi_index_name" sheetId="7" r:id="rId7"/>
-    <sheet name="both_name" sheetId="8" r:id="rId8"/>
-    <sheet name="both_name_skiprows" sheetId="10" r:id="rId9"/>
-    <sheet name="index_col_none" sheetId="13" r:id="rId10"/>
+    <sheet name="mi_index_blank_after_name" sheetId="14" r:id="rId8"/>
+    <sheet name="both_name" sheetId="8" r:id="rId9"/>
+    <sheet name="both_name_blank_after_mi_name" sheetId="15" r:id="rId10"/>
+    <sheet name="both_name_multiple_blanks" sheetId="16" r:id="rId11"/>
+    <sheet name="both_name_skiprows" sheetId="10" r:id="rId12"/>
+    <sheet name="index_col_none" sheetId="13" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="14">
   <si>
     <t>a</t>
   </si>
@@ -135,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -173,6 +176,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -546,9 +558,9 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -565,7 +577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -582,7 +594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -599,7 +611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -616,7 +628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -639,16 +651,423 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA9C600E-C910-4E4B-A937-81CED17EEF41}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="A1:F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2.5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>42005</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="16"/>
+      <c r="B5" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>3.5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>42006</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>4.5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>42007</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="16"/>
+      <c r="B7" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>5.5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>42008</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90541F65-2900-8245-80D1-E9A2DB31041E}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="15"/>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2.5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>42005</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="16"/>
+      <c r="B5" s="15"/>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>3.5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>42006</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>4.5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>42007</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="16"/>
+      <c r="B7" s="15"/>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>5.5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>42008</v>
+      </c>
+      <c r="F7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A3:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="16"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>2.5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>42005</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="16"/>
+      <c r="B7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>3.5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>42006</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>4.5</v>
+      </c>
+      <c r="E8" s="2">
+        <v>42007</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="16"/>
+      <c r="B9" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>5.5</v>
+      </c>
+      <c r="E9" s="2">
+        <v>42008</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC70534C-1941-4D3C-AD60-169D2BD8790A}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
@@ -662,7 +1081,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>12</v>
       </c>
@@ -676,7 +1095,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>1</v>
       </c>
@@ -690,7 +1109,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>1</v>
       </c>
@@ -718,20 +1137,20 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12" t="s">
+      <c r="B1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="12"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -746,7 +1165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -763,7 +1182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -780,7 +1199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -797,7 +1216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -829,9 +1248,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3" t="s">
@@ -847,7 +1266,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -867,7 +1286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
         <v>1</v>
@@ -885,7 +1304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -905,7 +1324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
         <v>1</v>
@@ -936,20 +1355,20 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" s="5"/>
-      <c r="C1" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12" t="s">
+      <c r="C1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="12"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" s="5"/>
       <c r="C2" s="5" t="s">
         <v>0</v>
@@ -964,8 +1383,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -984,8 +1403,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="16"/>
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
@@ -1002,8 +1421,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1022,8 +1441,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="16"/>
       <c r="B7" s="5" t="s">
         <v>1</v>
       </c>
@@ -1059,22 +1478,22 @@
       <selection sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12" t="s">
+      <c r="B1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="12"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1091,7 +1510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -1108,7 +1527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1125,7 +1544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1142,7 +1561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1176,22 +1595,22 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12" t="s">
+      <c r="B1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="12"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
@@ -1208,7 +1627,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>0</v>
       </c>
@@ -1225,7 +1644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>1</v>
       </c>
@@ -1242,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>2</v>
       </c>
@@ -1259,7 +1678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>3</v>
       </c>
@@ -1290,12 +1709,12 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F5"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
@@ -1315,8 +1734,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1335,8 +1754,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="16"/>
       <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1353,8 +1772,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -1373,8 +1792,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="16"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
@@ -1401,29 +1820,142 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ED35431-7858-4D4F-9852-3808836E5829}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2.5</v>
+      </c>
+      <c r="E2" s="2">
+        <v>42005</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="16"/>
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>3.5</v>
+      </c>
+      <c r="E3" s="2">
+        <v>42006</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>4.5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>42007</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="16"/>
+      <c r="B5" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>5.5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>42008</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F7" sqref="A1:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12" t="s">
+      <c r="C1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="12"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
@@ -1440,7 +1972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -1452,8 +1984,8 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -1472,8 +2004,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="16"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
@@ -1490,8 +2022,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -1510,8 +2042,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="16"/>
       <c r="B7" s="6" t="s">
         <v>1</v>
       </c>
@@ -1537,143 +2069,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A3:F9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="12"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>2.5</v>
-      </c>
-      <c r="E6" s="2">
-        <v>42005</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>3.5</v>
-      </c>
-      <c r="E7" s="2">
-        <v>42006</v>
-      </c>
-      <c r="F7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>4.5</v>
-      </c>
-      <c r="E8" s="2">
-        <v>42007</v>
-      </c>
-      <c r="F8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>5.5</v>
-      </c>
-      <c r="E9" s="2">
-        <v>42008</v>
-      </c>
-      <c r="F9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
BUG: read_excel failed with empty rows after MultiIndex header (#40649)
</commit_message>
<xml_diff>
--- a/pandas/tests/io/data/excel/testmultiindex.xlsx
+++ b/pandas/tests/io/data/excel/testmultiindex.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewzeitlin/Code/contrib/pandas-mzeitlin11/pandas/tests/io/data/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hawryla\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CD6934-D64C-2943-AF8E-713547E05FF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DC06E0-A119-495B-955B-C014FD6EA4B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29670" yWindow="435" windowWidth="22350" windowHeight="14805" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="single_column_name" sheetId="9" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="both_name_multiple_blanks" sheetId="16" r:id="rId11"/>
     <sheet name="both_name_skiprows" sheetId="10" r:id="rId12"/>
     <sheet name="index_col_none" sheetId="13" r:id="rId13"/>
+    <sheet name="mi_column_empty_rows" sheetId="17" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="14">
   <si>
     <t>a</t>
   </si>
@@ -86,7 +87,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +102,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -135,8 +141,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -187,8 +194,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{97F49660-B3B4-48EF-9E85-73FCFA1C086A}"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -558,9 +566,9 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -577,7 +585,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -594,7 +602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -611,7 +619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -628,7 +636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -658,9 +666,9 @@
       <selection activeCell="F7" sqref="A1:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="14" t="s">
         <v>6</v>
       </c>
@@ -673,7 +681,7 @@
       </c>
       <c r="F1" s="16"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
         <v>7</v>
       </c>
@@ -690,7 +698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -702,7 +710,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>4</v>
       </c>
@@ -720,7 +728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="14" t="s">
         <v>1</v>
@@ -738,7 +746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>5</v>
       </c>
@@ -758,7 +766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="14" t="s">
         <v>1</v>
@@ -791,13 +799,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90541F65-2900-8245-80D1-E9A2DB31041E}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="15" t="s">
         <v>6</v>
       </c>
@@ -810,7 +818,7 @@
       </c>
       <c r="F1" s="16"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="15" t="s">
         <v>7</v>
       </c>
@@ -827,7 +835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -839,7 +847,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>4</v>
       </c>
@@ -857,7 +865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="15"/>
       <c r="C5">
@@ -873,7 +881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>5</v>
       </c>
@@ -891,7 +899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="15"/>
       <c r="C7">
@@ -926,9 +934,9 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
@@ -941,7 +949,7 @@
       </c>
       <c r="F3" s="16"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
@@ -958,7 +966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
@@ -970,7 +978,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
@@ -990,7 +998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="9" t="s">
         <v>1</v>
@@ -1008,7 +1016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>5</v>
       </c>
@@ -1028,7 +1036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="9" t="s">
         <v>1</v>
@@ -1065,9 +1073,9 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>10</v>
       </c>
@@ -1081,7 +1089,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>12</v>
       </c>
@@ -1095,7 +1103,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <v>1</v>
       </c>
@@ -1109,7 +1117,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>1</v>
       </c>
@@ -1126,6 +1134,51 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C150B238-2309-4D4A-9A62-C0FE59966AB0}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1137,9 +1190,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="16" t="s">
         <v>4</v>
@@ -1150,7 +1203,7 @@
       </c>
       <c r="E1" s="16"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1165,7 +1218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0</v>
       </c>
@@ -1182,7 +1235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -1199,7 +1252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -1216,7 +1269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -1248,9 +1301,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3" t="s">
@@ -1266,7 +1319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1286,7 +1339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
         <v>1</v>
@@ -1304,7 +1357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1324,7 +1377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
         <v>1</v>
@@ -1355,9 +1408,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="5"/>
       <c r="C1" s="16" t="s">
         <v>4</v>
@@ -1368,7 +1421,7 @@
       </c>
       <c r="F1" s="16"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="5"/>
       <c r="C2" s="5" t="s">
         <v>0</v>
@@ -1383,7 +1436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>4</v>
       </c>
@@ -1403,7 +1456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="5" t="s">
         <v>1</v>
@@ -1421,7 +1474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>5</v>
       </c>
@@ -1441,7 +1494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="5" t="s">
         <v>1</v>
@@ -1478,9 +1531,9 @@
       <selection sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1493,7 +1546,7 @@
       </c>
       <c r="E1" s="16"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1510,7 +1563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -1527,7 +1580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1544,7 +1597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -1561,7 +1614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1595,9 +1648,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
@@ -1610,7 +1663,7 @@
       </c>
       <c r="E1" s="16"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
@@ -1627,7 +1680,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>0</v>
       </c>
@@ -1644,7 +1697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>1</v>
       </c>
@@ -1661,7 +1714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>2</v>
       </c>
@@ -1678,7 +1731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>3</v>
       </c>
@@ -1712,9 +1765,9 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
@@ -1734,7 +1787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>4</v>
       </c>
@@ -1754,7 +1807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="6" t="s">
         <v>1</v>
@@ -1772,7 +1825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>5</v>
       </c>
@@ -1792,7 +1845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
@@ -1827,9 +1880,9 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
@@ -1849,7 +1902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>4</v>
       </c>
@@ -1867,7 +1920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="12" t="s">
         <v>1</v>
@@ -1885,7 +1938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>5</v>
       </c>
@@ -1905,7 +1958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="12" t="s">
         <v>1</v>
@@ -1940,9 +1993,9 @@
       <selection activeCell="F7" sqref="A1:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>6</v>
       </c>
@@ -1955,7 +2008,7 @@
       </c>
       <c r="F1" s="16"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
@@ -1972,7 +2025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -1984,7 +2037,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>4</v>
       </c>
@@ -2004,7 +2057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
@@ -2022,7 +2075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>5</v>
       </c>
@@ -2042,7 +2095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="6" t="s">
         <v>1</v>

</xml_diff>